<commit_message>
File EBSCO Additional EC Servisbot TranslationsTest2.xlsx committed.
</commit_message>
<xml_diff>
--- a/de-hi-ko-ja-it-pt_br-zh_cn-fr-es-tr/EBSCO Additional EC Servisbot TranslationsTest2-en_us-de-hi-ko-ja-it-pt_br-zh_cn-fr-es-tr-C.xlsx
+++ b/de-hi-ko-ja-it-pt_br-zh_cn-fr-es-tr/EBSCO Additional EC Servisbot TranslationsTest2-en_us-de-hi-ko-ja-it-pt_br-zh_cn-fr-es-tr-C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\AppData\Roaming\memsource\mso-converter\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B788F4E-098C-412C-A389-7CDCE3113791}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5AE8319-6D90-41A9-9EDB-E8B524DD0CCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21060" windowHeight="10665" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21060" windowHeight="10665" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output-edit" sheetId="1" state="hidden" r:id="rId1"/>

</xml_diff>